<commit_message>
alles upgedatetd bis auf den Tep sensor da fehlt der stop button
</commit_message>
<xml_diff>
--- a/Weitere Dokumente/Pinbelegung.xlsx
+++ b/Weitere Dokumente/Pinbelegung.xlsx
@@ -248,10 +248,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -534,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -672,7 +671,7 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -686,7 +685,7 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -703,7 +702,7 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -936,7 +935,7 @@
       <c r="D26" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -953,7 +952,7 @@
       <c r="D27" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -970,7 +969,7 @@
       <c r="D28" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -987,7 +986,7 @@
       <c r="D29" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dokumentation Pinbelegung an aktuellen stand angepasst
</commit_message>
<xml_diff>
--- a/Weitere Dokumente/Pinbelegung.xlsx
+++ b/Weitere Dokumente/Pinbelegung.xlsx
@@ -194,9 +194,6 @@
     <t>AI2</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>UART RX</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>nicht Verbinden</t>
+  </si>
+  <si>
+    <t>Temperatursensor</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A2:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -685,7 +685,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,8 +732,8 @@
       <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="E14" t="s">
-        <v>56</v>
+      <c r="E14" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,13 +821,13 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,10 +844,10 @@
         <v>31</v>
       </c>
       <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
         <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -966,7 +966,7 @@
         <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>